<commit_message>
criado metodos de geração de arquivos json, sorteio de nomes sem repetição e interface grafica com kivy
</commit_message>
<xml_diff>
--- a/projteo/pkla.xlsx
+++ b/projteo/pkla.xlsx
@@ -362,7 +362,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2020-03-05</t>
+          <t>2020-03-12</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -389,7 +389,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-03-05</t>
+          <t>2020-03-12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -411,7 +411,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-03-08</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -438,7 +438,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-03-05</t>
+          <t>2020-03-12</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-03-08</t>
+          <t>2020-03-15</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -487,7 +487,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2020-03-12</t>
+          <t>2020-03-19</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2020-03-15</t>
+          <t>2020-03-22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -536,7 +536,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2020-03-19</t>
+          <t>2020-03-26</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2020-03-22</t>
+          <t>2020-03-29</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -585,7 +585,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2020-03-26</t>
+          <t>2020-04-02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -607,7 +607,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2020-03-29</t>
+          <t>2020-04-05</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2020-04-02</t>
+          <t>2020-04-09</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -656,7 +656,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2020-04-05</t>
+          <t>2020-04-12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -683,7 +683,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2020-04-09</t>
+          <t>2020-04-16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -705,7 +705,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2020-04-05</t>
+          <t>2020-04-12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">

</xml_diff>

<commit_message>
Inclui todos os exemplos fornecido pelo Marcos do forum python brasil
</commit_message>
<xml_diff>
--- a/projteo/pkla.xlsx
+++ b/projteo/pkla.xlsx
@@ -362,7 +362,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2020-03-12</t>
+          <t>2020-04-23</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -389,7 +389,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-03-12</t>
+          <t>2020-04-23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -409,11 +409,6 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2020-03-08</t>
-        </is>
-      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>['Leonardo Verzi', 'Renato Verzi']</t>
@@ -438,7 +433,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-03-12</t>
+          <t>2020-04-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -460,7 +455,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-03-15</t>
+          <t>2020-04-26</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -485,11 +480,6 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2020-03-19</t>
-        </is>
-      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>['Eduardo Ferraz', 'João Melo']</t>
@@ -509,7 +499,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2020-03-22</t>
+          <t>2020-05-03</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -536,7 +526,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2020-03-26</t>
+          <t>2020-05-07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -558,7 +548,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2020-03-29</t>
+          <t>2020-05-10</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -585,7 +575,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2020-04-02</t>
+          <t>2020-05-14</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -607,7 +597,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2020-04-05</t>
+          <t>2020-05-17</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -634,7 +624,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2020-04-09</t>
+          <t>2020-05-21</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -656,7 +646,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2020-04-12</t>
+          <t>2020-05-24</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -683,7 +673,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2020-04-16</t>
+          <t>2020-05-28</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -705,7 +695,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2020-04-12</t>
+          <t>2020-05-31</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">

</xml_diff>